<commit_message>
Update Master SW List via Streamlit on 2025-04-24T20:49:31.625399
</commit_message>
<xml_diff>
--- a/data/Master_SW_List.xlsx
+++ b/data/Master_SW_List.xlsx
@@ -553,11 +553,7 @@
           <t>68586439AD</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Testtttttt</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>#0: 24.24.20</t>
@@ -588,7 +584,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>68593292AC</t>
+          <t>68593292AA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>

</xml_diff>

<commit_message>
Update Master SW List via Streamlit on 2025-04-24T20:50:48.990234
</commit_message>
<xml_diff>
--- a/data/Master_SW_List.xlsx
+++ b/data/Master_SW_List.xlsx
@@ -584,10 +584,14 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>68593292AA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>68593292AC</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>#0: 24.39.00</t>
@@ -625,7 +629,11 @@
           <t>68593006AE</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>#0: 24.47.00</t>
@@ -659,7 +667,11 @@
           <t>68728746AB</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>#0: 25.7.00</t>

</xml_diff>

<commit_message>
Update Master SW List via Streamlit on 2025-04-25T11:44:56.026805
</commit_message>
<xml_diff>
--- a/data/Master_SW_List.xlsx
+++ b/data/Master_SW_List.xlsx
@@ -584,14 +584,10 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>68593292ACtest</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Test1</t>
-        </is>
-      </c>
+          <t>68593292AC</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>#0: 24.39.00</t>
@@ -629,11 +625,7 @@
           <t>68593006AE</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>test2</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>#0: 24.47.00</t>
@@ -667,11 +659,7 @@
           <t>68728746AB</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>test3</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>#0: 25.7.00</t>

</xml_diff>